<commit_message>
Sensitivity Analysis - Added CapacityCreditIncr
</commit_message>
<xml_diff>
--- a/projects/va_emerging_tech/data/sensitivityVariables_emerging_tech.xlsx
+++ b/projects/va_emerging_tech/data/sensitivityVariables_emerging_tech.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benne\PycharmProjects\coopercenter_temoatools\projects\va_emerging_tech\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66666E2B-7B91-460A-B63E-1F9650800DC0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A63AED6-2BF5-4778-A39B-F064B4DEA929}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="5" r:id="rId1"/>
@@ -497,7 +497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -927,7 +927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>